<commit_message>
Update Vignettes for DfReadDataFile, including split-plot design
devtools::test()
devtools::build_vignettes()
pkgdown::build_site()
</commit_message>
<xml_diff>
--- a/inst/extdata/toyFiles/ROC/rocCr.xlsx
+++ b/inst/extdata/toyFiles/ROC/rocCr.xlsx
@@ -1,17 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28421"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11110"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Dev/GitHub/RJafroc/inst/extdata/toyFiles/ROC/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1518C027-8B99-4141-85D8-5DA602E3AEDF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16420" yWindow="140" windowWidth="11380" windowHeight="10580" activeTab="1"/>
+    <workbookView xWindow="16420" yWindow="460" windowWidth="10000" windowHeight="10140" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FP" sheetId="2" r:id="rId1"/>
-    <sheet name="TRUTH" sheetId="1" r:id="rId2"/>
-    <sheet name="TP" sheetId="3" r:id="rId3"/>
+    <sheet name="TP" sheetId="3" r:id="rId2"/>
+    <sheet name="TRUTH" sheetId="1" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="140001"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -77,7 +83,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -141,6 +147,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -465,19 +479,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="4" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -491,7 +505,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -505,7 +519,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -519,7 +533,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -533,7 +547,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -547,7 +561,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -561,7 +575,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -575,7 +589,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
@@ -589,7 +603,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -603,7 +617,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -617,7 +631,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -631,7 +645,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
@@ -645,7 +659,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>9</v>
       </c>
@@ -659,7 +673,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>10</v>
       </c>
@@ -673,7 +687,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>10</v>
       </c>
@@ -687,7 +701,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>10</v>
       </c>
@@ -701,7 +715,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>6</v>
       </c>
@@ -715,7 +729,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>6</v>
       </c>
@@ -729,7 +743,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>6</v>
       </c>
@@ -743,7 +757,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>7</v>
       </c>
@@ -757,7 +771,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>7</v>
       </c>
@@ -771,7 +785,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>7</v>
       </c>
@@ -785,7 +799,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>8</v>
       </c>
@@ -799,7 +813,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>8</v>
       </c>
@@ -813,7 +827,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>8</v>
       </c>
@@ -827,7 +841,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>9</v>
       </c>
@@ -841,7 +855,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>9</v>
       </c>
@@ -855,7 +869,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>9</v>
       </c>
@@ -869,7 +883,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>10</v>
       </c>
@@ -883,7 +897,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>10</v>
       </c>
@@ -897,7 +911,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>10</v>
       </c>
@@ -925,269 +939,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F26"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="1" max="3" width="8.83203125" style="1"/>
-    <col min="4" max="4" width="13" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.33203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="8.83203125" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1">
-        <v>0</v>
-      </c>
-      <c r="C2" s="1">
-        <v>0</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1">
-        <v>0</v>
-      </c>
-      <c r="C3" s="1">
-        <v>0</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="1">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1">
-        <v>0</v>
-      </c>
-      <c r="C4" s="1">
-        <v>0</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4"/>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="1">
-        <v>70</v>
-      </c>
-      <c r="B5" s="1">
-        <v>1</v>
-      </c>
-      <c r="C5" s="1">
-        <v>1</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5"/>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="1">
-        <v>71</v>
-      </c>
-      <c r="B6" s="1">
-        <v>1</v>
-      </c>
-      <c r="C6" s="1">
-        <v>1</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F6"/>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="1">
-        <v>72</v>
-      </c>
-      <c r="B7" s="1">
-        <v>1</v>
-      </c>
-      <c r="C7" s="1">
-        <v>1</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F7"/>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="1">
-        <v>73</v>
-      </c>
-      <c r="B8" s="1">
-        <v>1</v>
-      </c>
-      <c r="C8" s="1">
-        <v>1</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F8"/>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="1">
-        <v>74</v>
-      </c>
-      <c r="B9" s="1">
-        <v>1</v>
-      </c>
-      <c r="C9" s="1">
-        <v>1</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F9"/>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="E10"/>
-      <c r="F10"/>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="E11"/>
-      <c r="F11"/>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="E12"/>
-      <c r="F12"/>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="E13"/>
-      <c r="F13"/>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="E14" s="2"/>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="E15" s="2"/>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="E16" s="2"/>
-    </row>
-    <row r="17" spans="5:5">
-      <c r="E17" s="2"/>
-    </row>
-    <row r="18" spans="5:5">
-      <c r="E18" s="2"/>
-    </row>
-    <row r="19" spans="5:5">
-      <c r="E19" s="2"/>
-    </row>
-    <row r="20" spans="5:5">
-      <c r="E20" s="2"/>
-    </row>
-    <row r="21" spans="5:5">
-      <c r="E21" s="2"/>
-    </row>
-    <row r="22" spans="5:5">
-      <c r="E22" s="2"/>
-    </row>
-    <row r="23" spans="5:5">
-      <c r="E23" s="2"/>
-    </row>
-    <row r="24" spans="5:5">
-      <c r="E24" s="2"/>
-    </row>
-    <row r="25" spans="5:5">
-      <c r="E25" s="2"/>
-    </row>
-    <row r="26" spans="5:5">
-      <c r="E26" s="2"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="5" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -1204,7 +968,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -1221,7 +985,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -1238,7 +1002,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -1255,7 +1019,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -1272,7 +1036,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -1289,7 +1053,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -1306,7 +1070,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
@@ -1323,7 +1087,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
@@ -1340,7 +1104,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>7</v>
       </c>
@@ -1357,7 +1121,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>7</v>
       </c>
@@ -1374,7 +1138,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>8</v>
       </c>
@@ -1391,7 +1155,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>8</v>
       </c>
@@ -1408,7 +1172,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>8</v>
       </c>
@@ -1425,7 +1189,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>8</v>
       </c>
@@ -1442,7 +1206,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>8</v>
       </c>
@@ -1459,7 +1223,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>9</v>
       </c>
@@ -1476,7 +1240,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>9</v>
       </c>
@@ -1493,7 +1257,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>9</v>
       </c>
@@ -1510,7 +1274,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>9</v>
       </c>
@@ -1527,7 +1291,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>9</v>
       </c>
@@ -1544,7 +1308,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>10</v>
       </c>
@@ -1561,7 +1325,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>10</v>
       </c>
@@ -1578,7 +1342,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>10</v>
       </c>
@@ -1595,7 +1359,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>10</v>
       </c>
@@ -1612,7 +1376,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>10</v>
       </c>
@@ -1629,7 +1393,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>6</v>
       </c>
@@ -1646,7 +1410,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>6</v>
       </c>
@@ -1663,7 +1427,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>6</v>
       </c>
@@ -1680,7 +1444,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>6</v>
       </c>
@@ -1697,7 +1461,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>6</v>
       </c>
@@ -1714,7 +1478,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>7</v>
       </c>
@@ -1731,7 +1495,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>7</v>
       </c>
@@ -1748,7 +1512,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>7</v>
       </c>
@@ -1765,7 +1529,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>7</v>
       </c>
@@ -1782,7 +1546,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>7</v>
       </c>
@@ -1799,7 +1563,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>8</v>
       </c>
@@ -1816,7 +1580,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>8</v>
       </c>
@@ -1833,7 +1597,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>8</v>
       </c>
@@ -1850,7 +1614,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>8</v>
       </c>
@@ -1867,7 +1631,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>8</v>
       </c>
@@ -1884,7 +1648,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
         <v>9</v>
       </c>
@@ -1901,7 +1665,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>9</v>
       </c>
@@ -1918,7 +1682,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="44" spans="1:5">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
         <v>9</v>
       </c>
@@ -1935,7 +1699,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
         <v>9</v>
       </c>
@@ -1952,7 +1716,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="46" spans="1:5">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
         <v>9</v>
       </c>
@@ -1969,7 +1733,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="47" spans="1:5">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
         <v>10</v>
       </c>
@@ -1986,7 +1750,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="1:5">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
         <v>10</v>
       </c>
@@ -2003,7 +1767,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="1:5">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
         <v>10</v>
       </c>
@@ -2020,7 +1784,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="50" spans="1:5">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
         <v>10</v>
       </c>
@@ -2037,7 +1801,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="51" spans="1:5">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
         <v>10</v>
       </c>
@@ -2065,4 +1829,254 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:F26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:F1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="3" width="8.83203125" style="1"/>
+    <col min="4" max="4" width="13" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="8.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>70</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1">
+        <v>1</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>71</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>72</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1</v>
+      </c>
+      <c r="C7" s="1">
+        <v>1</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>73</v>
+      </c>
+      <c r="B8" s="1">
+        <v>1</v>
+      </c>
+      <c r="C8" s="1">
+        <v>1</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>74</v>
+      </c>
+      <c r="B9" s="1">
+        <v>1</v>
+      </c>
+      <c r="C9" s="1">
+        <v>1</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E10"/>
+      <c r="F10"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E11"/>
+      <c r="F11"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E12"/>
+      <c r="F12"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E13"/>
+      <c r="F13"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E14" s="2"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E15" s="2"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E16" s="2"/>
+    </row>
+    <row r="17" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E17" s="2"/>
+    </row>
+    <row r="18" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E18" s="2"/>
+    </row>
+    <row r="19" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E19" s="2"/>
+    </row>
+    <row r="20" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E20" s="2"/>
+    </row>
+    <row r="21" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E21" s="2"/>
+    </row>
+    <row r="22" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E22" s="2"/>
+    </row>
+    <row r="23" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E23" s="2"/>
+    </row>
+    <row r="24" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E24" s="2"/>
+    </row>
+    <row r="25" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E25" s="2"/>
+    </row>
+    <row r="26" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E26" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>